<commit_message>
Corrección en excel de Renta Fija/Variable
El monto se presenta como un valor único, con una columna aparte que diga si es compra o venta, además de rescatar la comisión de la operación.
</commit_message>
<xml_diff>
--- a/Nevasa/Renta/20240822/20240822_nevasa_renta_results.xlsx
+++ b/Nevasa/Renta/20240822/20240822_nevasa_renta_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,12 +470,17 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>compra</t>
+          <t>monto</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>venta</t>
+          <t>tipo_instrumento</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>comision</t>
         </is>
       </c>
     </row>
@@ -507,7 +512,12 @@
       <c r="G2" t="n">
         <v>10879382</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -539,7 +549,12 @@
       <c r="G3" t="n">
         <v>1519368</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -569,10 +584,15 @@
         <v>8500</v>
       </c>
       <c r="G4" t="n">
+        <v>314272851</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
         <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>314272851</v>
       </c>
     </row>
     <row r="5">
@@ -601,10 +621,15 @@
         <v>1287</v>
       </c>
       <c r="G5" t="n">
+        <v>1519368</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
         <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1519368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>